<commit_message>
creates word and Excel documents with README file
</commit_message>
<xml_diff>
--- a/answers.xlsx
+++ b/answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\Downloads\בהד\תפיסות פיקוד\gaf_100\Mashov-Sagaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A1562B-592B-4777-AA49-CEDBD677E695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C130743A-F257-4277-B01D-5DD3639A6842}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,7 +716,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
a small bag fixed
</commit_message>
<xml_diff>
--- a/answers.xlsx
+++ b/answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\Downloads\בהד\תפיסות פיקוד\gaf_100\Mashov-Sagaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C130743A-F257-4277-B01D-5DD3639A6842}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D571316-A000-480D-A7DC-A390615F1CC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -328,9 +328,6 @@
     <t>אחלה גבר</t>
   </si>
   <si>
-    <t>תגובות קצרות נעלמות</t>
-  </si>
-  <si>
     <t>אחלה גבר! והכל+ אבל!</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t xml:space="preserve"> תיאורית - הצוערים התבקשו לפרט את נקודות החוזק והחולשה שזיהו בך כמפקד, בכל אחד מן התחומים. בשאלה הכללית, התבקשו הצוערים לנמק את הדירוג </t>
+  </si>
+  <si>
+    <t>מהווה דוגמה אישית</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1265,7 @@
         <v>80</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>81</v>
@@ -1365,10 +1365,10 @@
         <v>80</v>
       </c>
       <c r="D20" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>82</v>
@@ -1415,7 +1415,7 @@
         <v>90</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
if none of the above and another option is chosen the code now ignores none of the above
</commit_message>
<xml_diff>
--- a/answers.xlsx
+++ b/answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\Downloads\בהד\תפיסות פיקוד\gaf_100\Mashov-Sagaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524DFC64-CC14-4372-8413-125D62C9F695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E706EE89-EBC6-47CF-B391-019737D8C48F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="115">
   <si>
     <t>Timestamp</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>זהו זה נגמר הסיפור!</t>
+  </si>
+  <si>
+    <t>החלטי/ת, סמכותי/ת ובטוח/ה בעצמו/ה, אף אחד מההיגדים אינו נכון בעיניי</t>
   </si>
 </sst>
 </file>
@@ -903,7 +906,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1623,7 @@
         <v>94</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>95</v>
@@ -1629,7 +1632,7 @@
         <v>49</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>96</v>

</xml_diff>